<commit_message>
In Progress(PP: Gant Chart )
</commit_message>
<xml_diff>
--- a/Milestone1/Excel_Documents/Gantt chart.xlsx
+++ b/Milestone1/Excel_Documents/Gantt chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Courses\2810ICT\2024\2810-7810-workspace\Group_Project\M1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Luke/My Drive/Documents/07_Study/02_Bachelor Of Information Technology/Tri_2_2024/02_2810ICT_Software Tech/Assignment_01/SoftTech_Group_06/Milestone1/Excel_Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9675C1-8042-4DA2-BC81-E829931B8A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053C00BD-3028-8F4F-B1A2-BDDB79F89133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1665" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18400" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -37,87 +37,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>PERIODS</t>
-  </si>
-  <si>
-    <t>Activity 01</t>
-  </si>
-  <si>
-    <t>Activity 02</t>
-  </si>
-  <si>
-    <t>Activity 03</t>
-  </si>
-  <si>
-    <t>Activity 04</t>
-  </si>
-  <si>
-    <t>Activity 05</t>
-  </si>
-  <si>
-    <t>Activity 06</t>
-  </si>
-  <si>
-    <t>Activity 07</t>
-  </si>
-  <si>
-    <t>Activity 08</t>
-  </si>
-  <si>
-    <t>Activity 09</t>
-  </si>
-  <si>
-    <t>Activity 10</t>
-  </si>
-  <si>
-    <t>Activity 11</t>
-  </si>
-  <si>
-    <t>Activity 12</t>
-  </si>
-  <si>
-    <t>Activity 13</t>
-  </si>
-  <si>
-    <t>Activity 14</t>
-  </si>
-  <si>
-    <t>Activity 15</t>
-  </si>
-  <si>
-    <t>Activity 16</t>
-  </si>
-  <si>
-    <t>Activity 17</t>
-  </si>
-  <si>
-    <t>Activity 18</t>
-  </si>
-  <si>
-    <t>Activity 19</t>
-  </si>
-  <si>
-    <t>Activity 20</t>
-  </si>
-  <si>
-    <t>Activity 21</t>
-  </si>
-  <si>
-    <t>Activity 22</t>
-  </si>
-  <si>
-    <t>Activity 23</t>
-  </si>
-  <si>
-    <t>Activity 24</t>
-  </si>
-  <si>
-    <t>Activity 25</t>
-  </si>
-  <si>
-    <t>Activity 26</t>
   </si>
   <si>
     <r>
@@ -207,36 +129,6 @@
     <t>Plan Duration</t>
   </si>
   <si>
-    <t>Activity 27</t>
-  </si>
-  <si>
-    <t>Activity 28</t>
-  </si>
-  <si>
-    <t>Activity 29</t>
-  </si>
-  <si>
-    <t>Activity 30</t>
-  </si>
-  <si>
-    <t>Activity 31</t>
-  </si>
-  <si>
-    <t>Activity 32</t>
-  </si>
-  <si>
-    <t>Activity 33</t>
-  </si>
-  <si>
-    <t>Activity 34</t>
-  </si>
-  <si>
-    <t>Activity 35</t>
-  </si>
-  <si>
-    <t>Project Title</t>
-  </si>
-  <si>
     <t>Plan
 Start</t>
   </si>
@@ -262,13 +154,127 @@
   </si>
   <si>
     <t>Activity No. and Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nutra Graph </t>
+  </si>
+  <si>
+    <t>1. Initalisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2 Assign Project Manager </t>
+  </si>
+  <si>
+    <t>1.3 Assign Team Roles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Planning </t>
+  </si>
+  <si>
+    <t>3. Design</t>
+  </si>
+  <si>
+    <t>4. Software Development</t>
+  </si>
+  <si>
+    <t>4.2 GUI Development</t>
+  </si>
+  <si>
+    <t>4.3 Data Base Intergration</t>
+  </si>
+  <si>
+    <t>4.4 Database Algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.5 Pie &amp; Bar Graph Intergration </t>
+  </si>
+  <si>
+    <t>5. Testing &amp; QA</t>
+  </si>
+  <si>
+    <t>5.1 Intergration Testin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.2 User Acceptance Testing </t>
+  </si>
+  <si>
+    <t>5.3 Bug Fixes</t>
+  </si>
+  <si>
+    <t>6. Deployment</t>
+  </si>
+  <si>
+    <t>6.1 Document Handover</t>
+  </si>
+  <si>
+    <t>6.2 Software Deployment</t>
+  </si>
+  <si>
+    <t>W7</t>
+  </si>
+  <si>
+    <t>W8</t>
+  </si>
+  <si>
+    <t>W9</t>
+  </si>
+  <si>
+    <t>W10</t>
+  </si>
+  <si>
+    <t>W11</t>
+  </si>
+  <si>
+    <t>2.4 Create Gant Chart (PP:4)</t>
+  </si>
+  <si>
+    <t>2.3 Create WBS (PP:2)</t>
+  </si>
+  <si>
+    <t>2.2 Activity Definition Estimation (PP:3)</t>
+  </si>
+  <si>
+    <t>2.1 Create Project Plan (PP:1-4)</t>
+  </si>
+  <si>
+    <t>1.5 Define Project Scope (PP:1.3)</t>
+  </si>
+  <si>
+    <t>1.4 Define Stakeholders (PP:1.2)</t>
+  </si>
+  <si>
+    <t>1.1 Define Project Overview (PP:1)</t>
+  </si>
+  <si>
+    <t>3.2 Define User Requirments (SD:2)</t>
+  </si>
+  <si>
+    <t>3.3 Define Software Requirments (SD:2.2)</t>
+  </si>
+  <si>
+    <t>3.1 Define System Vision (SD:1)</t>
+  </si>
+  <si>
+    <t>3.4 Use Case's + Diagram (SD:2.3-2.4)</t>
+  </si>
+  <si>
+    <t>3.8 Wireframe Design (SD:4.2)</t>
+  </si>
+  <si>
+    <t>3.6 Structrual Design (SD:4.1)</t>
+  </si>
+  <si>
+    <t>3.5 Software Design &amp; Components (SD:3)</t>
+  </si>
+  <si>
+    <t>3.7 Detailed Design (SD:3.2.3)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -374,6 +380,13 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -565,7 +578,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -638,6 +651,33 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
@@ -650,32 +690,11 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1077,28 +1096,30 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BO39"/>
+  <dimension ref="B1:BO36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="AB23" sqref="AB23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="21.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="6.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="37" style="2" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.75" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.75" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.375" style="4" customWidth="1"/>
-    <col min="8" max="27" width="2.75" style="1"/>
-    <col min="42" max="42" width="2.75" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="4" customWidth="1"/>
+    <col min="8" max="17" width="4" style="1" customWidth="1"/>
+    <col min="18" max="27" width="4.5" style="1" customWidth="1"/>
+    <col min="28" max="28" width="4.83203125" customWidth="1"/>
+    <col min="29" max="59" width="4.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="11" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -1106,53 +1127,53 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="2:67" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+    <row r="2" spans="2:67" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="21" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="H2" s="12">
         <v>1</v>
       </c>
       <c r="J2" s="13"/>
-      <c r="K2" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="32"/>
+      <c r="K2" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="28"/>
       <c r="P2" s="14"/>
-      <c r="Q2" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="32"/>
+      <c r="Q2" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="28"/>
       <c r="U2" s="15"/>
-      <c r="V2" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="36"/>
+      <c r="V2" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="31"/>
+      <c r="X2" s="31"/>
+      <c r="Y2" s="32"/>
       <c r="Z2" s="16"/>
-      <c r="AA2" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB2" s="35"/>
-      <c r="AC2" s="35"/>
-      <c r="AD2" s="35"/>
-      <c r="AE2" s="35"/>
-      <c r="AF2" s="35"/>
-      <c r="AG2" s="36"/>
+      <c r="AA2" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="31"/>
+      <c r="AC2" s="31"/>
+      <c r="AD2" s="31"/>
+      <c r="AE2" s="31"/>
+      <c r="AF2" s="31"/>
+      <c r="AG2" s="32"/>
       <c r="AH2" s="17"/>
       <c r="AI2" s="19" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="AJ2" s="20"/>
       <c r="AK2" s="20"/>
@@ -1162,24 +1183,24 @@
       <c r="AO2" s="20"/>
       <c r="AP2" s="20"/>
     </row>
-    <row r="3" spans="2:67" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>46</v>
+    <row r="3" spans="2:67" s="9" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>10</v>
       </c>
       <c r="H3" s="18" t="s">
         <v>0</v>
@@ -1189,28 +1210,41 @@
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
+      <c r="N3" s="38" t="s">
+        <v>31</v>
+      </c>
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
       <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
+      <c r="U3" s="38" t="s">
+        <v>32</v>
+      </c>
       <c r="V3" s="8"/>
       <c r="W3" s="8"/>
       <c r="X3" s="8"/>
       <c r="Y3" s="8"/>
       <c r="Z3" s="8"/>
       <c r="AA3" s="8"/>
-    </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
+      <c r="AB3" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI3" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="AP3" s="38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="35"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1392,458 +1426,558 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0</v>
-      </c>
-      <c r="G5" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5">
+        <v>4</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+      <c r="G6" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
         <v>2</v>
       </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
       <c r="G7" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
+        <v>2</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
+      <c r="G8" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
         <v>4</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
       <c r="G9" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5">
+        <v>4</v>
+      </c>
+      <c r="F10" s="5">
+        <v>2</v>
+      </c>
       <c r="G10" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="23" t="s">
-        <v>7</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="37" t="s">
+        <v>17</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="22"/>
+    </row>
+    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="C12" s="5">
+        <v>2</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5">
+        <v>4</v>
+      </c>
+      <c r="F12" s="5">
+        <v>3</v>
+      </c>
       <c r="G12" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="C13" s="5">
+        <v>2</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5">
+        <v>4</v>
+      </c>
+      <c r="F13" s="5">
+        <v>1</v>
+      </c>
       <c r="G13" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="C14" s="6">
+        <v>3</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5">
+        <v>5</v>
+      </c>
+      <c r="F14" s="5">
+        <v>1</v>
+      </c>
       <c r="G14" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="C15" s="5">
+        <v>3</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5">
+        <v>5</v>
+      </c>
+      <c r="F15" s="5">
+        <v>2</v>
+      </c>
       <c r="G15" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="23" t="s">
-        <v>12</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="37" t="s">
+        <v>18</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="22"/>
+    </row>
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+        <v>45</v>
+      </c>
+      <c r="C17" s="5">
+        <v>4</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1</v>
+      </c>
+      <c r="E17" s="5">
+        <v>4</v>
+      </c>
+      <c r="F17" s="5">
+        <v>1</v>
+      </c>
       <c r="G17" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="C18" s="5">
+        <v>4</v>
+      </c>
+      <c r="D18" s="5">
+        <v>1</v>
+      </c>
+      <c r="E18" s="5">
+        <v>5</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1</v>
+      </c>
       <c r="G18" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="C19" s="5">
+        <v>4</v>
+      </c>
+      <c r="D19" s="5">
+        <v>1</v>
+      </c>
+      <c r="E19" s="5">
+        <v>5</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1</v>
+      </c>
       <c r="G19" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="C20" s="5">
+        <v>5</v>
+      </c>
+      <c r="D20" s="5">
+        <v>1</v>
+      </c>
+      <c r="E20" s="5">
+        <v>5</v>
+      </c>
+      <c r="F20" s="5">
+        <v>2</v>
+      </c>
       <c r="G20" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+        <v>49</v>
+      </c>
+      <c r="C21" s="5">
+        <v>5</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1</v>
+      </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="C22" s="5">
+        <v>6</v>
+      </c>
+      <c r="D22" s="5">
+        <v>1</v>
+      </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="C23" s="5">
+        <v>6</v>
+      </c>
+      <c r="D23" s="5">
+        <v>1</v>
+      </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="C24" s="5">
+        <v>7</v>
+      </c>
+      <c r="D24" s="5">
+        <v>1</v>
+      </c>
+      <c r="E24" s="5">
+        <v>5</v>
+      </c>
+      <c r="F24" s="5">
+        <v>1</v>
+      </c>
       <c r="G24" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="23" t="s">
-        <v>21</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="37" t="s">
+        <v>19</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="22"/>
+    </row>
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="C26" s="5">
+        <v>8</v>
+      </c>
+      <c r="D26" s="5">
+        <v>7</v>
+      </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="C27" s="5">
+        <v>15</v>
+      </c>
+      <c r="D27" s="5">
+        <v>6</v>
+      </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="C28" s="5">
+        <v>21</v>
+      </c>
+      <c r="D28" s="5">
+        <v>6</v>
+      </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="C29" s="5">
+        <v>27</v>
+      </c>
+      <c r="D29" s="5">
+        <v>3</v>
+      </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="23" t="s">
-        <v>26</v>
+    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="37" t="s">
+        <v>24</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
-      <c r="G30" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G30" s="22"/>
+    </row>
+    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="C31" s="5">
+        <v>30</v>
+      </c>
+      <c r="D31" s="5">
+        <v>1</v>
+      </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C32" s="5">
+        <v>31</v>
+      </c>
+      <c r="D32" s="5">
+        <v>1</v>
+      </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="C33" s="5">
+        <v>32</v>
+      </c>
+      <c r="D33" s="5">
+        <v>3</v>
+      </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="23" t="s">
-        <v>35</v>
+    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="37" t="s">
+        <v>28</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
-      <c r="G34" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G34" s="22"/>
+    </row>
+    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="C35" s="5">
+        <v>35</v>
+      </c>
+      <c r="D35" s="5">
+        <v>1</v>
+      </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="C36" s="5">
+        <v>35</v>
+      </c>
+      <c r="D36" s="5">
+        <v>1</v>
+      </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="22">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:BO4">
     <cfRule type="expression" dxfId="8" priority="8">
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:BO39">
+  <conditionalFormatting sqref="H5:BO36">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added( 4.Gantt Chart, 3. Activity Def Estimations)
</commit_message>
<xml_diff>
--- a/Milestone1/Excel_Documents/Gantt chart.xlsx
+++ b/Milestone1/Excel_Documents/Gantt chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Luke/My Drive/Documents/07_Study/02_Bachelor Of Information Technology/Tri_2_2024/02_2810ICT_Software Tech/Assignment_01/SoftTech_Group_06/Milestone1/Excel_Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053C00BD-3028-8F4F-B1A2-BDDB79F89133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F8E0EB-C67D-0845-97EC-A251D4B09097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18400" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18400" yWindow="-21100" windowWidth="51200" windowHeight="19740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -177,18 +177,6 @@
     <t>4. Software Development</t>
   </si>
   <si>
-    <t>4.2 GUI Development</t>
-  </si>
-  <si>
-    <t>4.3 Data Base Intergration</t>
-  </si>
-  <si>
-    <t>4.4 Database Algorithm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.5 Pie &amp; Bar Graph Intergration </t>
-  </si>
-  <si>
     <t>5. Testing &amp; QA</t>
   </si>
   <si>
@@ -268,6 +256,18 @@
   </si>
   <si>
     <t>3.7 Detailed Design (SD:3.2.3)</t>
+  </si>
+  <si>
+    <t>4.1 GUI Development</t>
+  </si>
+  <si>
+    <t>4.2 Data Base Intergration</t>
+  </si>
+  <si>
+    <t>4.3 Database Algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.4 Pie &amp; Bar Graph Intergration </t>
   </si>
 </sst>
 </file>
@@ -309,6 +309,7 @@
       <sz val="12"/>
       <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -651,6 +652,12 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -688,12 +695,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1098,8 +1099,8 @@
   </sheetPr>
   <dimension ref="B1:BO36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AB23" sqref="AB23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1115,6 +1116,7 @@
     <col min="18" max="27" width="4.5" style="1" customWidth="1"/>
     <col min="28" max="28" width="4.83203125" customWidth="1"/>
     <col min="29" max="59" width="4.5" customWidth="1"/>
+    <col min="60" max="67" width="3.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
@@ -1128,11 +1130,11 @@
       <c r="G1" s="10"/>
     </row>
     <row r="2" spans="2:67" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
       <c r="G2" s="21" t="s">
         <v>11</v>
       </c>
@@ -1140,37 +1142,37 @@
         <v>1</v>
       </c>
       <c r="J2" s="13"/>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="28"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="30"/>
       <c r="P2" s="14"/>
-      <c r="Q2" s="26" t="s">
+      <c r="Q2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="28"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="30"/>
       <c r="U2" s="15"/>
-      <c r="V2" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="32"/>
+      <c r="V2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="34"/>
       <c r="Z2" s="16"/>
-      <c r="AA2" s="30" t="s">
+      <c r="AA2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="31"/>
-      <c r="AD2" s="31"/>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="32"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
+      <c r="AF2" s="33"/>
+      <c r="AG2" s="34"/>
       <c r="AH2" s="17"/>
       <c r="AI2" s="19" t="s">
         <v>3</v>
@@ -1184,22 +1186,22 @@
       <c r="AP2" s="20"/>
     </row>
     <row r="3" spans="2:67" s="9" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="26" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="18" t="s">
@@ -1210,8 +1212,8 @@
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
-      <c r="N3" s="38" t="s">
-        <v>31</v>
+      <c r="N3" s="25" t="s">
+        <v>27</v>
       </c>
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
@@ -1219,8 +1221,8 @@
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
       <c r="T3" s="8"/>
-      <c r="U3" s="38" t="s">
-        <v>32</v>
+      <c r="U3" s="25" t="s">
+        <v>28</v>
       </c>
       <c r="V3" s="8"/>
       <c r="W3" s="8"/>
@@ -1228,23 +1230,23 @@
       <c r="Y3" s="8"/>
       <c r="Z3" s="8"/>
       <c r="AA3" s="8"/>
-      <c r="AB3" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI3" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="AP3" s="38" t="s">
-        <v>35</v>
+      <c r="AB3" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI3" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP3" s="25" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="35"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1427,7 +1429,7 @@
       </c>
     </row>
     <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="24" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="5"/>
@@ -1438,7 +1440,7 @@
     </row>
     <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="23" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C6" s="5">
         <v>1</v>
@@ -1498,7 +1500,7 @@
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="23" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C9" s="5">
         <v>1</v>
@@ -1518,7 +1520,7 @@
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="23" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C10" s="5">
         <v>1</v>
@@ -1537,7 +1539,7 @@
       </c>
     </row>
     <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="24" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="5"/>
@@ -1548,7 +1550,7 @@
     </row>
     <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="23" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C12" s="5">
         <v>2</v>
@@ -1568,7 +1570,7 @@
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C13" s="5">
         <v>2</v>
@@ -1588,7 +1590,7 @@
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="23" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C14" s="6">
         <v>3</v>
@@ -1608,7 +1610,7 @@
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="23" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C15" s="5">
         <v>3</v>
@@ -1627,7 +1629,7 @@
       </c>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="5"/>
@@ -1638,7 +1640,7 @@
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="23" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C17" s="5">
         <v>4</v>
@@ -1658,7 +1660,7 @@
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="23" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C18" s="5">
         <v>4</v>
@@ -1678,7 +1680,7 @@
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="23" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C19" s="5">
         <v>4</v>
@@ -1698,7 +1700,7 @@
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="23" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C20" s="5">
         <v>5</v>
@@ -1718,7 +1720,7 @@
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="23" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C21" s="5">
         <v>5</v>
@@ -1726,15 +1728,19 @@
       <c r="D21" s="5">
         <v>1</v>
       </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+      <c r="E21" s="5">
+        <v>7</v>
+      </c>
+      <c r="F21" s="5">
+        <v>1</v>
+      </c>
       <c r="G21" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="23" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C22" s="5">
         <v>6</v>
@@ -1742,15 +1748,19 @@
       <c r="D22" s="5">
         <v>1</v>
       </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+      <c r="E22" s="5">
+        <v>7</v>
+      </c>
+      <c r="F22" s="5">
+        <v>1</v>
+      </c>
       <c r="G22" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="23" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C23" s="5">
         <v>6</v>
@@ -1758,15 +1768,19 @@
       <c r="D23" s="5">
         <v>1</v>
       </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="E23" s="5">
+        <v>7</v>
+      </c>
+      <c r="F23" s="5">
+        <v>1</v>
+      </c>
       <c r="G23" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="23" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C24" s="5">
         <v>7</v>
@@ -1785,7 +1799,7 @@
       </c>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="24" t="s">
         <v>19</v>
       </c>
       <c r="C25" s="5"/>
@@ -1796,7 +1810,7 @@
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="23" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C26" s="5">
         <v>8</v>
@@ -1812,7 +1826,7 @@
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="23" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="C27" s="5">
         <v>15</v>
@@ -1828,7 +1842,7 @@
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="23" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="C28" s="5">
         <v>21</v>
@@ -1844,7 +1858,7 @@
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="23" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="C29" s="5">
         <v>27</v>
@@ -1859,8 +1873,8 @@
       </c>
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="37" t="s">
-        <v>24</v>
+      <c r="B30" s="24" t="s">
+        <v>20</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -1870,7 +1884,7 @@
     </row>
     <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="23" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C31" s="5">
         <v>30</v>
@@ -1886,7 +1900,7 @@
     </row>
     <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="23" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C32" s="5">
         <v>31</v>
@@ -1902,7 +1916,7 @@
     </row>
     <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="23" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C33" s="5">
         <v>32</v>
@@ -1917,8 +1931,8 @@
       </c>
     </row>
     <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="37" t="s">
-        <v>28</v>
+      <c r="B34" s="24" t="s">
+        <v>24</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -1928,7 +1942,7 @@
     </row>
     <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="23" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C35" s="5">
         <v>35</v>
@@ -1944,7 +1958,7 @@
     </row>
     <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="23" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C36" s="5">
         <v>35</v>

</xml_diff>